<commit_message>
luban excel export fixed
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/Datas/BuffConfig.xlsx
+++ b/Unity/Assets/Config/Excel/Datas/BuffConfig.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>##var</t>
   </si>
@@ -232,9 +232,6 @@
     <t>攻击+50%</t>
   </si>
   <si>
-    <t>[1]</t>
-  </si>
-  <si>
     <t>BuffEffect02</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>攻击-100</t>
   </si>
   <si>
-    <t>[2]</t>
-  </si>
-  <si>
     <t>BuffEffect05</t>
   </si>
   <si>
@@ -286,7 +280,7 @@
     <t>速度-100%</t>
   </si>
   <si>
-    <t>[2,3]</t>
+    <t>2,3</t>
   </si>
   <si>
     <t>BuffEffect08</t>
@@ -316,7 +310,7 @@
     <t>回复200点/3秒</t>
   </si>
   <si>
-    <t>[1,4]</t>
+    <t>1,4</t>
   </si>
   <si>
     <t>BuffEffect11</t>
@@ -359,7 +353,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,13 +541,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1034,7 +1021,7 @@
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1422,7 +1409,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="M4" sqref="M4:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1710,13 +1697,13 @@
       <c r="L5" s="10">
         <v>0</v>
       </c>
-      <c r="M5" s="10" t="s">
-        <v>49</v>
+      <c r="M5" s="10">
+        <v>1</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="10">
         <v>100</v>
@@ -1730,10 +1717,10 @@
         <v>8003</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
@@ -1757,15 +1744,15 @@
       <c r="L6" s="10">
         <v>0</v>
       </c>
-      <c r="M6" s="10" t="s">
-        <v>49</v>
+      <c r="M6" s="10">
+        <v>1</v>
       </c>
       <c r="N6" s="10">
         <v>1</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="10">
         <v>100</v>
@@ -1779,10 +1766,10 @@
         <v>8004</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="10">
         <v>1</v>
@@ -1806,15 +1793,15 @@
       <c r="L7" s="10">
         <v>0</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>49</v>
+      <c r="M7" s="10">
+        <v>1</v>
       </c>
       <c r="N7" s="10">
         <v>1</v>
       </c>
       <c r="O7" s="10"/>
       <c r="P7" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q7" s="10">
         <v>100</v>
@@ -1828,10 +1815,10 @@
         <v>8005</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="E8" s="10">
         <v>1</v>
@@ -1855,15 +1842,15 @@
       <c r="L8" s="10">
         <v>0</v>
       </c>
-      <c r="M8" s="10" t="s">
-        <v>58</v>
+      <c r="M8" s="10">
+        <v>2</v>
       </c>
       <c r="N8" s="10">
         <v>2</v>
       </c>
       <c r="O8" s="10"/>
       <c r="P8" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q8" s="10">
         <v>100</v>
@@ -1877,10 +1864,10 @@
         <v>8006</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="10">
         <v>1</v>
@@ -1904,15 +1891,15 @@
       <c r="L9" s="10">
         <v>0</v>
       </c>
-      <c r="M9" s="10" t="s">
-        <v>58</v>
+      <c r="M9" s="10">
+        <v>2</v>
       </c>
       <c r="N9" s="10">
         <v>2</v>
       </c>
       <c r="O9" s="10"/>
       <c r="P9" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q9" s="10">
         <v>100</v>
@@ -1926,10 +1913,10 @@
         <v>8007</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="10">
         <v>1</v>
@@ -1953,13 +1940,13 @@
       <c r="L10" s="10">
         <v>0</v>
       </c>
-      <c r="M10" s="10" t="s">
-        <v>49</v>
+      <c r="M10" s="10">
+        <v>1</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q10" s="10">
         <v>100</v>
@@ -1973,10 +1960,10 @@
         <v>8008</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11" s="10">
         <v>1</v>
@@ -2001,12 +1988,12 @@
         <v>0</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q11" s="10">
         <v>100</v>
@@ -2020,10 +2007,10 @@
         <v>8009</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="10">
         <v>1</v>
@@ -2049,13 +2036,13 @@
       <c r="L12" s="10">
         <v>0</v>
       </c>
-      <c r="M12" s="10" t="s">
-        <v>58</v>
+      <c r="M12" s="10">
+        <v>2</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q12" s="10">
         <v>100</v>
@@ -2069,10 +2056,10 @@
         <v>8010</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E13" s="10">
         <v>1</v>
@@ -2098,13 +2085,13 @@
       <c r="L13" s="10">
         <v>0</v>
       </c>
-      <c r="M13" s="10" t="s">
-        <v>58</v>
+      <c r="M13" s="10">
+        <v>2</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="P13" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q13" s="10">
         <v>100</v>
@@ -2118,10 +2105,10 @@
         <v>8011</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E14" s="10">
         <v>1</v>
@@ -2148,12 +2135,12 @@
         <v>0</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Q14" s="10">
         <v>100</v>
@@ -2167,10 +2154,10 @@
         <v>8012</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E15" s="10">
         <v>1</v>
@@ -2197,12 +2184,12 @@
         <v>0</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q15" s="10">
         <v>100</v>
@@ -2216,10 +2203,10 @@
         <v>8013</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="10">
         <v>1</v>
@@ -2246,12 +2233,12 @@
         <v>0</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q16" s="10">
         <v>100</v>
@@ -2265,10 +2252,10 @@
         <v>8014</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E17" s="10">
         <v>1</v>
@@ -2295,12 +2282,12 @@
         <v>0</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q17" s="10">
         <v>100</v>

</xml_diff>

<commit_message>
Battle System Refactoring : buff system
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/Datas/BuffConfig.xlsx
+++ b/Unity/Assets/Config/Excel/Datas/BuffConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23370" windowHeight="13770"/>
+    <workbookView windowWidth="22080" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Buff" sheetId="1" r:id="rId1"/>
@@ -33,30 +33,7 @@
     <author>cgm</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>cgm:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-单位：毫秒
--1表示无限时间</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U3" authorId="0">
+    <comment ref="L3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>##var</t>
   </si>
@@ -97,54 +74,27 @@
     <t>Desc</t>
   </si>
   <si>
-    <t>BuffType</t>
-  </si>
-  <si>
-    <t>NumericType</t>
-  </si>
-  <si>
-    <t>NumericValue</t>
+    <t>StartEvents</t>
+  </si>
+  <si>
+    <t>EndEvents</t>
   </si>
   <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>Interval</t>
-  </si>
-  <si>
-    <t>AddType</t>
-  </si>
-  <si>
-    <t>MaxNum</t>
-  </si>
-  <si>
-    <t>ReduceType</t>
-  </si>
-  <si>
-    <t>Tags</t>
+    <t>TriggerInterval</t>
+  </si>
+  <si>
+    <t>TriggerEvents</t>
+  </si>
+  <si>
+    <t>MaxLayer</t>
   </si>
   <si>
     <t>Goup</t>
   </si>
   <si>
-    <t>EffectRoot</t>
-  </si>
-  <si>
-    <t>EffectRes</t>
-  </si>
-  <si>
-    <t>EffectScale</t>
-  </si>
-  <si>
-    <t>TriggerEffectRoot</t>
-  </si>
-  <si>
-    <t>TriggerEffectRes</t>
-  </si>
-  <si>
-    <t>TriggerEffectScale</t>
-  </si>
-  <si>
     <t>##type</t>
   </si>
   <si>
@@ -169,13 +119,10 @@
     <t>备注</t>
   </si>
   <si>
-    <t>效果类型</t>
-  </si>
-  <si>
-    <t>效果参数</t>
-  </si>
-  <si>
-    <t>效果值</t>
+    <t>开始事件</t>
+  </si>
+  <si>
+    <t>结束事件</t>
   </si>
   <si>
     <t>持续时间</t>
@@ -184,163 +131,91 @@
     <t>触发间隔</t>
   </si>
   <si>
-    <t>叠加方式</t>
+    <t>触发事件id</t>
   </si>
   <si>
     <t>最大叠加层数</t>
   </si>
   <si>
-    <t>减少方式</t>
-  </si>
-  <si>
-    <t>标签</t>
-  </si>
-  <si>
     <t>分组</t>
   </si>
   <si>
-    <t>特效挂点</t>
-  </si>
-  <si>
-    <t>特效</t>
-  </si>
-  <si>
-    <t>特效缩放(100倍)</t>
-  </si>
-  <si>
-    <t>触发时的特效挂点</t>
-  </si>
-  <si>
-    <t>触发时的特效</t>
-  </si>
-  <si>
-    <t>触发时的特效缩放</t>
-  </si>
-  <si>
     <t>测试-标记buff</t>
   </si>
   <si>
     <t>纯标记</t>
   </si>
   <si>
-    <t>BuffEffect01</t>
-  </si>
-  <si>
     <t>测试-加攻击%</t>
   </si>
   <si>
     <t>攻击+50%</t>
   </si>
   <si>
-    <t>BuffEffect02</t>
-  </si>
-  <si>
     <t>测试-加攻击</t>
   </si>
   <si>
     <t>攻击+100</t>
   </si>
   <si>
-    <t>BuffEffect03</t>
-  </si>
-  <si>
     <t>攻击+200</t>
   </si>
   <si>
-    <t>BuffEffect04</t>
-  </si>
-  <si>
     <t>测试-减攻击</t>
   </si>
   <si>
     <t>攻击-100</t>
   </si>
   <si>
-    <t>BuffEffect05</t>
-  </si>
-  <si>
     <t>攻击-300</t>
   </si>
   <si>
-    <t>BuffEffect06</t>
-  </si>
-  <si>
     <t>测试-加速</t>
   </si>
   <si>
     <t>速度+50</t>
   </si>
   <si>
-    <t>BuffEffect07</t>
-  </si>
-  <si>
     <t>测试-减速%</t>
   </si>
   <si>
     <t>速度-100%</t>
   </si>
   <si>
-    <t>2,3</t>
-  </si>
-  <si>
-    <t>BuffEffect08</t>
-  </si>
-  <si>
     <t>测试-持续伤害</t>
   </si>
   <si>
     <t>500伤害/秒</t>
   </si>
   <si>
-    <t>BuffEffect09</t>
-  </si>
-  <si>
     <t>测试-持续伤害%</t>
   </si>
   <si>
     <t>血量上限5%伤害/5秒</t>
   </si>
   <si>
-    <t>BuffEffect10</t>
-  </si>
-  <si>
     <t>测试-持续回血</t>
   </si>
   <si>
     <t>回复200点/3秒</t>
   </si>
   <si>
-    <t>1,4</t>
-  </si>
-  <si>
-    <t>BuffEffect11</t>
-  </si>
-  <si>
     <t>测试-持续回血%</t>
   </si>
   <si>
     <t>回复血量上限10%点/3秒</t>
   </si>
   <si>
-    <t>BuffEffect12</t>
-  </si>
-  <si>
     <t>测试-持续回护盾</t>
   </si>
   <si>
     <t>加100盾/2秒</t>
   </si>
   <si>
-    <t>BuffEffect13</t>
-  </si>
-  <si>
     <t>测试-持续回护盾%</t>
   </si>
   <si>
     <t>加10%盾/2秒</t>
-  </si>
-  <si>
-    <t>BuffEffect14</t>
   </si>
 </sst>
 </file>
@@ -1406,10 +1281,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M17"/>
+      <selection activeCell="L1" sqref="L$1:Q$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1418,26 +1293,18 @@
     <col min="2" max="2" width="9" style="7"/>
     <col min="3" max="3" width="17.625" style="7" customWidth="1"/>
     <col min="4" max="4" width="23.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="12.7083333333333" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="9.875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="9.25" style="7" customWidth="1"/>
-    <col min="11" max="11" width="12.875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="13.75" style="7" customWidth="1"/>
-    <col min="13" max="13" width="15" style="7" customWidth="1"/>
-    <col min="14" max="14" width="11.875" style="8" customWidth="1"/>
-    <col min="15" max="15" width="13.125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="21.125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="19" style="7" customWidth="1"/>
-    <col min="18" max="19" width="20.625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="17.25" style="7" customWidth="1"/>
-    <col min="21" max="21" width="18.875" style="7" customWidth="1"/>
-    <col min="22" max="16384" width="9" style="7"/>
+    <col min="5" max="5" width="14" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11.625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15" style="7" customWidth="1"/>
+    <col min="10" max="10" width="12.875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="11.875" style="8" customWidth="1"/>
+    <col min="12" max="12" width="18.875" style="7" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="16.5" spans="1:20">
+    <row r="1" s="2" customFormat="1" ht="16.5" spans="1:11">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1471,835 +1338,490 @@
       <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
+    </row>
+    <row r="2" s="2" customFormat="1" ht="16.5" spans="1:11">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="D2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="F2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="16.5" spans="1:12">
+      <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" s="2" customFormat="1" ht="16.5" spans="1:20">
-      <c r="A2" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" s="2" customFormat="1" ht="16.5" spans="1:21">
-      <c r="A3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="4" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B4" s="10">
         <v>8001</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="10">
+        <v>27</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10">
         <v>0</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10">
-        <v>15000</v>
-      </c>
-      <c r="I4" s="10"/>
       <c r="J4" s="10">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
         <v>1</v>
       </c>
-      <c r="L4" s="10">
-        <v>0</v>
-      </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q4" s="10">
-        <v>100</v>
-      </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-    </row>
-    <row r="5" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B5" s="10">
         <v>8002</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E5" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F5" s="10">
+        <v>5000</v>
+      </c>
+      <c r="G5" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
         <v>1</v>
       </c>
-      <c r="F5" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G5" s="10">
-        <v>5000</v>
-      </c>
-      <c r="H5" s="10">
-        <v>10000</v>
-      </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10">
-        <v>1</v>
-      </c>
-      <c r="L5" s="10">
-        <v>0</v>
-      </c>
-      <c r="M5" s="10">
-        <v>1</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q5" s="10">
-        <v>100</v>
-      </c>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-    </row>
-    <row r="6" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B6" s="10">
         <v>8003</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E6" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F6" s="10">
+        <v>100</v>
+      </c>
+      <c r="G6" s="10">
+        <v>12000</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
         <v>1</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G6" s="10">
-        <v>100</v>
-      </c>
-      <c r="H6" s="10">
-        <v>12000</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10">
-        <v>0</v>
       </c>
       <c r="K6" s="10">
         <v>1</v>
       </c>
-      <c r="L6" s="10">
-        <v>0</v>
-      </c>
-      <c r="M6" s="10">
-        <v>1</v>
-      </c>
-      <c r="N6" s="10">
-        <v>1</v>
-      </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q6" s="10">
-        <v>100</v>
-      </c>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-    </row>
-    <row r="7" s="2" customFormat="1" ht="16.5" spans="2:20">
+    </row>
+    <row r="7" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B7" s="10">
         <v>8004</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E7" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F7" s="10">
+        <v>200</v>
+      </c>
+      <c r="G7" s="10">
+        <v>12000</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
         <v>1</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G7" s="10">
-        <v>200</v>
-      </c>
-      <c r="H7" s="10">
-        <v>12000</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10">
-        <v>0</v>
       </c>
       <c r="K7" s="10">
         <v>1</v>
       </c>
-      <c r="L7" s="10">
-        <v>0</v>
-      </c>
-      <c r="M7" s="10">
-        <v>1</v>
-      </c>
-      <c r="N7" s="10">
-        <v>1</v>
-      </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q7" s="10">
-        <v>100</v>
-      </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-    </row>
-    <row r="8" s="2" customFormat="1" ht="16.5" spans="2:20">
+    </row>
+    <row r="8" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B8" s="10">
         <v>8005</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E8" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F8" s="10">
+        <v>-100</v>
+      </c>
+      <c r="G8" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
         <v>1</v>
       </c>
-      <c r="F8" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G8" s="10">
-        <v>-100</v>
-      </c>
-      <c r="H8" s="10">
-        <v>10000</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10">
-        <v>0</v>
-      </c>
       <c r="K8" s="10">
-        <v>1</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0</v>
-      </c>
-      <c r="M8" s="10">
         <v>2</v>
       </c>
-      <c r="N8" s="10">
-        <v>2</v>
-      </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>100</v>
-      </c>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-    </row>
-    <row r="9" s="2" customFormat="1" ht="16.5" spans="2:20">
+    </row>
+    <row r="9" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B9" s="10">
         <v>8006</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="E9" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F9" s="10">
+        <v>-300</v>
+      </c>
+      <c r="G9" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
         <v>1</v>
       </c>
-      <c r="F9" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G9" s="10">
-        <v>-300</v>
-      </c>
-      <c r="H9" s="10">
-        <v>10000</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10">
-        <v>0</v>
-      </c>
       <c r="K9" s="10">
-        <v>1</v>
-      </c>
-      <c r="L9" s="10">
-        <v>0</v>
-      </c>
-      <c r="M9" s="10">
         <v>2</v>
       </c>
-      <c r="N9" s="10">
-        <v>2</v>
-      </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>100</v>
-      </c>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-    </row>
-    <row r="10" s="2" customFormat="1" ht="16.5" spans="2:20">
+    </row>
+    <row r="10" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B10" s="10">
         <v>8007</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E10" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F10" s="10">
+        <v>50</v>
+      </c>
+      <c r="G10" s="10">
+        <v>5000</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
         <v>1</v>
       </c>
-      <c r="F10" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G10" s="10">
-        <v>50</v>
-      </c>
-      <c r="H10" s="10">
-        <v>5000</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10">
-        <v>0</v>
-      </c>
-      <c r="K10" s="10">
-        <v>1</v>
-      </c>
-      <c r="L10" s="10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="10">
-        <v>1</v>
-      </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q10" s="10">
-        <v>100</v>
-      </c>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-    </row>
-    <row r="11" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B11" s="10">
         <v>8008</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E11" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F11" s="10">
+        <v>-10000</v>
+      </c>
+      <c r="G11" s="10">
+        <v>7500</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10">
         <v>1</v>
       </c>
-      <c r="F11" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G11" s="10">
-        <v>-10000</v>
-      </c>
-      <c r="H11" s="10">
-        <v>7500</v>
-      </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10">
-        <v>0</v>
-      </c>
-      <c r="K11" s="10">
-        <v>1</v>
-      </c>
-      <c r="L11" s="10">
-        <v>0</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q11" s="10">
-        <v>100</v>
-      </c>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-    </row>
-    <row r="12" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B12" s="10">
         <v>8009</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="E12" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F12" s="10">
+        <v>500</v>
+      </c>
+      <c r="G12" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1000</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
         <v>1</v>
       </c>
-      <c r="F12" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G12" s="10">
-        <v>500</v>
-      </c>
-      <c r="H12" s="10">
-        <v>10000</v>
-      </c>
-      <c r="I12" s="10">
-        <v>1000</v>
-      </c>
-      <c r="J12" s="10">
-        <v>0</v>
-      </c>
-      <c r="K12" s="10">
-        <v>1</v>
-      </c>
-      <c r="L12" s="10">
-        <v>0</v>
-      </c>
-      <c r="M12" s="10">
-        <v>2</v>
-      </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q12" s="10">
-        <v>100</v>
-      </c>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-    </row>
-    <row r="13" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B13" s="10">
         <v>8010</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="E13" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F13" s="10">
+        <v>500</v>
+      </c>
+      <c r="G13" s="10">
+        <v>25000</v>
+      </c>
+      <c r="H13" s="10">
+        <v>5000</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
         <v>1</v>
       </c>
-      <c r="F13" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G13" s="10">
-        <v>500</v>
-      </c>
-      <c r="H13" s="10">
-        <v>25000</v>
-      </c>
-      <c r="I13" s="10">
-        <v>5000</v>
-      </c>
-      <c r="J13" s="10">
-        <v>0</v>
-      </c>
-      <c r="K13" s="10">
-        <v>1</v>
-      </c>
-      <c r="L13" s="10">
-        <v>0</v>
-      </c>
-      <c r="M13" s="10">
-        <v>2</v>
-      </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>100</v>
-      </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-    </row>
-    <row r="14" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B14" s="10">
         <v>8011</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="E14" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F14" s="10">
+        <v>200</v>
+      </c>
+      <c r="G14" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H14" s="10">
+        <v>3000</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
         <v>1</v>
       </c>
-      <c r="F14" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G14" s="10">
-        <v>200</v>
-      </c>
-      <c r="H14" s="10">
-        <v>15000</v>
-      </c>
-      <c r="I14" s="10">
-        <v>3000</v>
-      </c>
-      <c r="J14" s="10">
-        <v>0</v>
-      </c>
-      <c r="K14" s="10">
-        <v>1</v>
-      </c>
-      <c r="L14" s="10">
-        <v>0</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>100</v>
-      </c>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-    </row>
-    <row r="15" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B15" s="10">
         <v>8012</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="E15" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H15" s="10">
+        <v>3000</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
         <v>1</v>
       </c>
-      <c r="F15" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G15" s="10">
-        <v>1000</v>
-      </c>
-      <c r="H15" s="10">
-        <v>15000</v>
-      </c>
-      <c r="I15" s="10">
-        <v>3000</v>
-      </c>
-      <c r="J15" s="10">
-        <v>0</v>
-      </c>
-      <c r="K15" s="10">
-        <v>1</v>
-      </c>
-      <c r="L15" s="10">
-        <v>0</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q15" s="10">
-        <v>100</v>
-      </c>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B16" s="10">
         <v>8013</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="E16" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F16" s="10">
+        <v>100</v>
+      </c>
+      <c r="G16" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H16" s="10">
+        <v>2000</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10">
         <v>1</v>
       </c>
-      <c r="F16" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G16" s="10">
-        <v>100</v>
-      </c>
-      <c r="H16" s="10">
-        <v>10000</v>
-      </c>
-      <c r="I16" s="10">
-        <v>2000</v>
-      </c>
-      <c r="J16" s="10">
-        <v>0</v>
-      </c>
-      <c r="K16" s="10">
-        <v>1</v>
-      </c>
-      <c r="L16" s="10">
-        <v>0</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q16" s="10">
-        <v>100</v>
-      </c>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-    </row>
-    <row r="17" s="2" customFormat="1" ht="16.5" spans="2:20">
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" s="2" customFormat="1" ht="16.5" spans="2:11">
       <c r="B17" s="10">
         <v>8014</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="E17" s="10">
+        <v>1001</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1000</v>
+      </c>
+      <c r="G17" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H17" s="10">
+        <v>2000</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
         <v>1</v>
       </c>
-      <c r="F17" s="10">
-        <v>1001</v>
-      </c>
-      <c r="G17" s="10">
-        <v>1000</v>
-      </c>
-      <c r="H17" s="10">
-        <v>10000</v>
-      </c>
-      <c r="I17" s="10">
-        <v>2000</v>
-      </c>
-      <c r="J17" s="10">
-        <v>0</v>
-      </c>
-      <c r="K17" s="10">
-        <v>1</v>
-      </c>
-      <c r="L17" s="10">
-        <v>0</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q17" s="10">
-        <v>100</v>
-      </c>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-    </row>
-    <row r="18" spans="6:8">
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="5:7">
+      <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>